<commit_message>
Set null to reserved word.You can use it in cell of sheet.
</commit_message>
<xml_diff>
--- a/test1/wb1.xlsx
+++ b/test1/wb1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13940" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="96">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -376,6 +376,10 @@
   </si>
   <si>
     <t>__name__</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>null</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -441,8 +445,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="81">
+  <cellStyleXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -540,7 +546,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="81">
+  <cellStyles count="83">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -581,6 +587,7 @@
     <cellStyle name="超链接" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -621,6 +628,7 @@
     <cellStyle name="访问过的超链接" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -952,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1266,7 +1274,9 @@
       <c r="C7" s="4">
         <v>234</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="E7" s="4">
         <v>43</v>
       </c>
@@ -1314,9 +1324,6 @@
       </c>
       <c r="C8" s="4">
         <v>13</v>
-      </c>
-      <c r="D8" s="4">
-        <v>123</v>
       </c>
       <c r="E8" s="4">
         <v>32</v>
@@ -1894,7 +1901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Auto decide type for value in cell.
</commit_message>
<xml_diff>
--- a/test1/wb1.xlsx
+++ b/test1/wb1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="102">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -380,6 +380,30 @@
   </si>
   <si>
     <t>null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>auto</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -445,8 +469,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="83">
+  <cellStyleXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -546,7 +572,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="83">
+  <cellStyles count="85">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -588,6 +614,7 @@
     <cellStyle name="超链接" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -629,6 +656,7 @@
     <cellStyle name="访问过的超链接" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -958,10 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S34"/>
+  <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -977,7 +1005,7 @@
     <col min="14" max="17" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:20">
       <c r="A1" s="3" t="s">
         <v>40</v>
       </c>
@@ -1018,7 +1046,7 @@
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:20">
       <c r="A2" s="4" t="s">
         <v>39</v>
       </c>
@@ -1049,7 +1077,7 @@
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
     </row>
-    <row r="3" spans="1:19" s="1" customFormat="1">
+    <row r="3" spans="1:20" s="1" customFormat="1">
       <c r="A3" s="3" t="s">
         <v>41</v>
       </c>
@@ -1102,7 +1130,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="2" customFormat="1">
+    <row r="4" spans="1:20" s="2" customFormat="1">
       <c r="A4" s="5" t="s">
         <v>94</v>
       </c>
@@ -1154,8 +1182,11 @@
       <c r="Q4" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="5" spans="1:19">
+      <c r="R4" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
       <c r="A5" s="4">
         <v>10001</v>
       </c>
@@ -1207,11 +1238,14 @@
       <c r="Q5" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="S5" s="2" t="s">
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="T5" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:20">
       <c r="A6" s="4">
         <v>10002</v>
       </c>
@@ -1263,8 +1297,11 @@
       <c r="Q6" s="4" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="7" spans="1:19">
+      <c r="R6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
       <c r="A7" s="4">
         <v>10003</v>
       </c>
@@ -1314,8 +1351,11 @@
       <c r="Q7" s="4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="8" spans="1:19">
+      <c r="R7">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
       <c r="A8" s="4">
         <v>10004</v>
       </c>
@@ -1362,8 +1402,11 @@
       <c r="Q8" s="4" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="9" spans="1:19">
+      <c r="R8">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
       <c r="A9" s="4">
         <v>10005</v>
       </c>
@@ -1415,8 +1458,11 @@
       <c r="Q9" s="4" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="10" spans="1:19">
+      <c r="R9" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
       <c r="A10" s="4">
         <v>10006</v>
       </c>
@@ -1464,8 +1510,11 @@
       <c r="Q10" s="4" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="11" spans="1:19">
+      <c r="R10" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
       <c r="A11" s="4">
         <v>10007</v>
       </c>
@@ -1515,8 +1564,11 @@
       <c r="Q11" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="12" spans="1:19">
+      <c r="R11" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
       <c r="A12" s="4" t="s">
         <v>43</v>
       </c>
@@ -1566,8 +1618,11 @@
       <c r="Q12" s="4" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="13" spans="1:19">
+      <c r="R12" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
       <c r="A13" s="4">
         <v>10009</v>
       </c>
@@ -1619,8 +1674,11 @@
       <c r="Q13" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="14" spans="1:19">
+      <c r="R13" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1639,7 +1697,7 @@
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:20">
       <c r="A15" s="4" t="s">
         <v>37</v>
       </c>
@@ -1660,7 +1718,7 @@
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:20">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>

</xml_diff>

<commit_message>
In singlebook model,referenced sheet do not output
</commit_message>
<xml_diff>
--- a/test1/wb1.xlsx
+++ b/test1/wb1.xlsx
@@ -988,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="V18" sqref="V18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1256,7 +1256,8 @@
         <v>11</v>
       </c>
       <c r="D6" s="4">
-        <v>123</v>
+        <f>C5+C6</f>
+        <v>21</v>
       </c>
       <c r="E6" s="4">
         <v>32</v>

</xml_diff>